<commit_message>
model was over fitting so changed parameters
</commit_message>
<xml_diff>
--- a/Data_Analysis_Report.xlsx
+++ b/Data_Analysis_Report.xlsx
@@ -8,9 +8,10 @@
   </bookViews>
   <sheets>
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="DataFrame_Head" sheetId="1" state="visible" r:id="rId1"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Model_Metrics" sheetId="2" state="visible" r:id="rId2"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Correlation_Matrix" sheetId="3" state="visible" r:id="rId3"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Descriptive_Statistics" sheetId="4" state="visible" r:id="rId4"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Full_DataFrame" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Model_Metrics" sheetId="3" state="visible" r:id="rId3"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Correlation_Matrix" sheetId="4" state="visible" r:id="rId4"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Descriptive_Statistics" sheetId="5" state="visible" r:id="rId5"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -839,7 +840,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E2"/>
+  <dimension ref="A1:S63"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -850,45 +851,3756 @@
     <row r="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
-          <t>Mean Squared Error</t>
+          <t>ID</t>
         </is>
       </c>
       <c r="B1" s="1" t="inlineStr">
         <is>
-          <t>R-squared Score</t>
+          <t>Large_BP</t>
         </is>
       </c>
       <c r="C1" s="1" t="inlineStr">
         <is>
-          <t>Precision</t>
+          <t>Large_ROE</t>
         </is>
       </c>
       <c r="D1" s="1" t="inlineStr">
         <is>
-          <t>Recall</t>
+          <t>Large_SP</t>
         </is>
       </c>
       <c r="E1" s="1" t="inlineStr">
         <is>
-          <t>F1 Score</t>
+          <t>Large_Return_Rate_Last_Quarter</t>
+        </is>
+      </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
+          <t>Large_Market_Value</t>
+        </is>
+      </c>
+      <c r="G1" s="1" t="inlineStr">
+        <is>
+          <t>Small_Systematic_Risk</t>
+        </is>
+      </c>
+      <c r="H1" s="1" t="inlineStr">
+        <is>
+          <t>Annual_Return</t>
+        </is>
+      </c>
+      <c r="I1" s="1" t="inlineStr">
+        <is>
+          <t>Excess_Return</t>
+        </is>
+      </c>
+      <c r="J1" s="1" t="inlineStr">
+        <is>
+          <t>Systematic_Risk</t>
+        </is>
+      </c>
+      <c r="K1" s="1" t="inlineStr">
+        <is>
+          <t>Total_Risk</t>
+        </is>
+      </c>
+      <c r="L1" s="1" t="inlineStr">
+        <is>
+          <t>Abs_Win_Rate</t>
+        </is>
+      </c>
+      <c r="M1" s="1" t="inlineStr">
+        <is>
+          <t>Rel_Win_Rate</t>
+        </is>
+      </c>
+      <c r="N1" s="1" t="inlineStr">
+        <is>
+          <t>Annual_Return_Normalized</t>
+        </is>
+      </c>
+      <c r="O1" s="1" t="inlineStr">
+        <is>
+          <t>Excess_Return_Normalized</t>
+        </is>
+      </c>
+      <c r="P1" s="1" t="inlineStr">
+        <is>
+          <t>Systematic_Risk_Normalized</t>
+        </is>
+      </c>
+      <c r="Q1" s="1" t="inlineStr">
+        <is>
+          <t>Total_Risk_Normalized</t>
+        </is>
+      </c>
+      <c r="R1" s="1" t="inlineStr">
+        <is>
+          <t>Abs_Win_Rate_Normalized</t>
+        </is>
+      </c>
+      <c r="S1" s="1" t="inlineStr">
+        <is>
+          <t>Rel_Win_Rate_Normalized</t>
         </is>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="n">
-        <v>1.074318524048438e-06</v>
+        <v>2</v>
       </c>
       <c r="B2" t="n">
-        <v>0.9998999871635186</v>
+        <v>0</v>
       </c>
       <c r="C2" t="n">
         <v>1</v>
       </c>
       <c r="D2" t="n">
+        <v>0</v>
+      </c>
+      <c r="E2" t="n">
+        <v>0</v>
+      </c>
+      <c r="F2" t="n">
+        <v>0</v>
+      </c>
+      <c r="G2" t="n">
+        <v>0</v>
+      </c>
+      <c r="H2" t="n">
+        <v>0.143</v>
+      </c>
+      <c r="I2" t="n">
+        <v>0.01</v>
+      </c>
+      <c r="J2" t="n">
+        <v>1.17</v>
+      </c>
+      <c r="K2" t="n">
+        <v>0.108</v>
+      </c>
+      <c r="L2" t="n">
+        <v>0.663</v>
+      </c>
+      <c r="M2" t="n">
+        <v>0.65</v>
+      </c>
+      <c r="N2" t="n">
+        <v>0.5497115767632317</v>
+      </c>
+      <c r="O2" t="n">
+        <v>0.4875951550466297</v>
+      </c>
+      <c r="P2" t="n">
+        <v>0.5715793247407004</v>
+      </c>
+      <c r="Q2" t="n">
+        <v>0.4122310840579945</v>
+      </c>
+      <c r="R2" t="n">
+        <v>0.5199999999999999</v>
+      </c>
+      <c r="S2" t="n">
+        <v>0.7647058823529413</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="n">
+        <v>3</v>
+      </c>
+      <c r="B3" t="n">
+        <v>0</v>
+      </c>
+      <c r="C3" t="n">
+        <v>0</v>
+      </c>
+      <c r="D3" t="n">
         <v>1</v>
       </c>
-      <c r="E2" t="n">
+      <c r="E3" t="n">
+        <v>0</v>
+      </c>
+      <c r="F3" t="n">
+        <v>0</v>
+      </c>
+      <c r="G3" t="n">
+        <v>0</v>
+      </c>
+      <c r="H3" t="n">
+        <v>0.173</v>
+      </c>
+      <c r="I3" t="n">
+        <v>0.018</v>
+      </c>
+      <c r="J3" t="n">
+        <v>1.3</v>
+      </c>
+      <c r="K3" t="n">
+        <v>0.144</v>
+      </c>
+      <c r="L3" t="n">
+        <v>0.638</v>
+      </c>
+      <c r="M3" t="n">
+        <v>0.513</v>
+      </c>
+      <c r="N3" t="n">
+        <v>0.692625436280919</v>
+      </c>
+      <c r="O3" t="n">
+        <v>0.6298950110931354</v>
+      </c>
+      <c r="P3" t="n">
+        <v>0.70305137902405</v>
+      </c>
+      <c r="Q3" t="n">
+        <v>0.7568794273144732</v>
+      </c>
+      <c r="R3" t="n">
+        <v>0.4399999999999998</v>
+      </c>
+      <c r="S3" t="n">
+        <v>0.376470588235294</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="n">
+        <v>4</v>
+      </c>
+      <c r="B4" t="n">
+        <v>0</v>
+      </c>
+      <c r="C4" t="n">
+        <v>0</v>
+      </c>
+      <c r="D4" t="n">
+        <v>0</v>
+      </c>
+      <c r="E4" t="n">
         <v>1</v>
+      </c>
+      <c r="F4" t="n">
+        <v>0</v>
+      </c>
+      <c r="G4" t="n">
+        <v>0</v>
+      </c>
+      <c r="H4" t="n">
+        <v>0.096</v>
+      </c>
+      <c r="I4" t="n">
+        <v>-0.002</v>
+      </c>
+      <c r="J4" t="n">
+        <v>1.39</v>
+      </c>
+      <c r="K4" t="n">
+        <v>0.144</v>
+      </c>
+      <c r="L4" t="n">
+        <v>0.613</v>
+      </c>
+      <c r="M4" t="n">
+        <v>0.475</v>
+      </c>
+      <c r="N4" t="n">
+        <v>0.3243513889099982</v>
+      </c>
+      <c r="O4" t="n">
+        <v>0.2556340505025017</v>
+      </c>
+      <c r="P4" t="n">
+        <v>0.8</v>
+      </c>
+      <c r="Q4" t="n">
+        <v>0.756046465789155</v>
+      </c>
+      <c r="R4" t="n">
+        <v>0.3600000000000001</v>
+      </c>
+      <c r="S4" t="n">
+        <v>0.2705882352941176</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="n">
+        <v>5</v>
+      </c>
+      <c r="B5" t="n">
+        <v>0</v>
+      </c>
+      <c r="C5" t="n">
+        <v>0</v>
+      </c>
+      <c r="D5" t="n">
+        <v>0</v>
+      </c>
+      <c r="E5" t="n">
+        <v>0</v>
+      </c>
+      <c r="F5" t="n">
+        <v>1</v>
+      </c>
+      <c r="G5" t="n">
+        <v>0</v>
+      </c>
+      <c r="H5" t="n">
+        <v>0.096</v>
+      </c>
+      <c r="I5" t="n">
+        <v>0.001</v>
+      </c>
+      <c r="J5" t="n">
+        <v>1.04</v>
+      </c>
+      <c r="K5" t="n">
+        <v>0.08699999999999999</v>
+      </c>
+      <c r="L5" t="n">
+        <v>0.725</v>
+      </c>
+      <c r="M5" t="n">
+        <v>0.538</v>
+      </c>
+      <c r="N5" t="n">
+        <v>0.326614905519037</v>
+      </c>
+      <c r="O5" t="n">
+        <v>0.306500583264615</v>
+      </c>
+      <c r="P5" t="n">
+        <v>0.4324519177394552</v>
+      </c>
+      <c r="Q5" t="n">
+        <v>0.2092889005050929</v>
+      </c>
+      <c r="R5" t="n">
+        <v>0.72</v>
+      </c>
+      <c r="S5" t="n">
+        <v>0.4470588235294117</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="n">
+        <v>6</v>
+      </c>
+      <c r="B6" t="n">
+        <v>0</v>
+      </c>
+      <c r="C6" t="n">
+        <v>0</v>
+      </c>
+      <c r="D6" t="n">
+        <v>0</v>
+      </c>
+      <c r="E6" t="n">
+        <v>0</v>
+      </c>
+      <c r="F6" t="n">
+        <v>0</v>
+      </c>
+      <c r="G6" t="n">
+        <v>1</v>
+      </c>
+      <c r="H6" t="n">
+        <v>0.07000000000000001</v>
+      </c>
+      <c r="I6" t="n">
+        <v>-0.005</v>
+      </c>
+      <c r="J6" t="n">
+        <v>1.1</v>
+      </c>
+      <c r="K6" t="n">
+        <v>0.11</v>
+      </c>
+      <c r="L6" t="n">
+        <v>0.5629999999999999</v>
+      </c>
+      <c r="M6" t="n">
+        <v>0.463</v>
+      </c>
+      <c r="N6" t="n">
+        <v>0.2</v>
+      </c>
+      <c r="O6" t="n">
+        <v>0.2</v>
+      </c>
+      <c r="P6" t="n">
+        <v>0.4908823220030348</v>
+      </c>
+      <c r="Q6" t="n">
+        <v>0.4290628603730675</v>
+      </c>
+      <c r="R6" t="n">
+        <v>0.2</v>
+      </c>
+      <c r="S6" t="n">
+        <v>0.2352941176470588</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="n">
+        <v>7</v>
+      </c>
+      <c r="B7" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="C7" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="D7" t="n">
+        <v>0</v>
+      </c>
+      <c r="E7" t="n">
+        <v>0</v>
+      </c>
+      <c r="F7" t="n">
+        <v>0</v>
+      </c>
+      <c r="G7" t="n">
+        <v>0</v>
+      </c>
+      <c r="H7" t="n">
+        <v>0.195</v>
+      </c>
+      <c r="I7" t="n">
+        <v>0.026</v>
+      </c>
+      <c r="J7" t="n">
+        <v>0.97</v>
+      </c>
+      <c r="K7" t="n">
+        <v>0.105</v>
+      </c>
+      <c r="L7" t="n">
+        <v>0.738</v>
+      </c>
+      <c r="M7" t="n">
+        <v>0.638</v>
+      </c>
+      <c r="N7" t="n">
+        <v>0.8</v>
+      </c>
+      <c r="O7" t="n">
+        <v>0.8</v>
+      </c>
+      <c r="P7" t="n">
+        <v>0.3597522371815644</v>
+      </c>
+      <c r="Q7" t="n">
+        <v>0.3751911696122572</v>
+      </c>
+      <c r="R7" t="n">
+        <v>0.7600000000000002</v>
+      </c>
+      <c r="S7" t="n">
+        <v>0.7294117647058822</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="n">
+        <v>8</v>
+      </c>
+      <c r="B8" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="C8" t="n">
+        <v>0</v>
+      </c>
+      <c r="D8" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="E8" t="n">
+        <v>0</v>
+      </c>
+      <c r="F8" t="n">
+        <v>0</v>
+      </c>
+      <c r="G8" t="n">
+        <v>0</v>
+      </c>
+      <c r="H8" t="n">
+        <v>0.164</v>
+      </c>
+      <c r="I8" t="n">
+        <v>0.016</v>
+      </c>
+      <c r="J8" t="n">
+        <v>1.32</v>
+      </c>
+      <c r="K8" t="n">
+        <v>0.149</v>
+      </c>
+      <c r="L8" t="n">
+        <v>0.65</v>
+      </c>
+      <c r="M8" t="n">
+        <v>0.513</v>
+      </c>
+      <c r="N8" t="n">
+        <v>0.6521860403953194</v>
+      </c>
+      <c r="O8" t="n">
+        <v>0.594190452739228</v>
+      </c>
+      <c r="P8" t="n">
+        <v>0.7236552703825667</v>
+      </c>
+      <c r="Q8" t="n">
+        <v>0.7971945455765044</v>
+      </c>
+      <c r="R8" t="n">
+        <v>0.4800000000000001</v>
+      </c>
+      <c r="S8" t="n">
+        <v>0.376470588235294</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="n">
+        <v>9</v>
+      </c>
+      <c r="B9" t="n">
+        <v>0</v>
+      </c>
+      <c r="C9" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="D9" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="E9" t="n">
+        <v>0</v>
+      </c>
+      <c r="F9" t="n">
+        <v>0</v>
+      </c>
+      <c r="G9" t="n">
+        <v>0</v>
+      </c>
+      <c r="H9" t="n">
+        <v>0.185</v>
+      </c>
+      <c r="I9" t="n">
+        <v>0.022</v>
+      </c>
+      <c r="J9" t="n">
+        <v>1.06</v>
+      </c>
+      <c r="K9" t="n">
+        <v>0.109</v>
+      </c>
+      <c r="L9" t="n">
+        <v>0.675</v>
+      </c>
+      <c r="M9" t="n">
+        <v>0.65</v>
+      </c>
+      <c r="N9" t="n">
+        <v>0.7506206889941092</v>
+      </c>
+      <c r="O9" t="n">
+        <v>0.7211401110626023</v>
+      </c>
+      <c r="P9" t="n">
+        <v>0.4542097650936622</v>
+      </c>
+      <c r="Q9" t="n">
+        <v>0.418337611575535</v>
+      </c>
+      <c r="R9" t="n">
+        <v>0.5600000000000001</v>
+      </c>
+      <c r="S9" t="n">
+        <v>0.7647058823529413</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="n">
+        <v>10</v>
+      </c>
+      <c r="B10" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="C10" t="n">
+        <v>0</v>
+      </c>
+      <c r="D10" t="n">
+        <v>0</v>
+      </c>
+      <c r="E10" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="F10" t="n">
+        <v>0</v>
+      </c>
+      <c r="G10" t="n">
+        <v>0</v>
+      </c>
+      <c r="H10" t="n">
+        <v>0.15</v>
+      </c>
+      <c r="I10" t="n">
+        <v>0.015</v>
+      </c>
+      <c r="J10" t="n">
+        <v>1.05</v>
+      </c>
+      <c r="K10" t="n">
+        <v>0.113</v>
+      </c>
+      <c r="L10" t="n">
+        <v>0.7</v>
+      </c>
+      <c r="M10" t="n">
+        <v>0.513</v>
+      </c>
+      <c r="N10" t="n">
+        <v>0.5853214994439921</v>
+      </c>
+      <c r="O10" t="n">
+        <v>0.5871479040678567</v>
+      </c>
+      <c r="P10" t="n">
+        <v>0.4386408413573779</v>
+      </c>
+      <c r="Q10" t="n">
+        <v>0.4597882167053142</v>
+      </c>
+      <c r="R10" t="n">
+        <v>0.6399999999999999</v>
+      </c>
+      <c r="S10" t="n">
+        <v>0.376470588235294</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="n">
+        <v>11</v>
+      </c>
+      <c r="B11" t="n">
+        <v>0</v>
+      </c>
+      <c r="C11" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="D11" t="n">
+        <v>0</v>
+      </c>
+      <c r="E11" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="F11" t="n">
+        <v>0</v>
+      </c>
+      <c r="G11" t="n">
+        <v>0</v>
+      </c>
+      <c r="H11" t="n">
+        <v>0.159</v>
+      </c>
+      <c r="I11" t="n">
+        <v>0.015</v>
+      </c>
+      <c r="J11" t="n">
+        <v>1.17</v>
+      </c>
+      <c r="K11" t="n">
+        <v>0.115</v>
+      </c>
+      <c r="L11" t="n">
+        <v>0.675</v>
+      </c>
+      <c r="M11" t="n">
+        <v>0.638</v>
+      </c>
+      <c r="N11" t="n">
+        <v>0.6267327393505735</v>
+      </c>
+      <c r="O11" t="n">
+        <v>0.573724695421814</v>
+      </c>
+      <c r="P11" t="n">
+        <v>0.5635112843469086</v>
+      </c>
+      <c r="Q11" t="n">
+        <v>0.473207630009196</v>
+      </c>
+      <c r="R11" t="n">
+        <v>0.5600000000000001</v>
+      </c>
+      <c r="S11" t="n">
+        <v>0.7294117647058822</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="n">
+        <v>12</v>
+      </c>
+      <c r="B12" t="n">
+        <v>0</v>
+      </c>
+      <c r="C12" t="n">
+        <v>0</v>
+      </c>
+      <c r="D12" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="E12" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="F12" t="n">
+        <v>0</v>
+      </c>
+      <c r="G12" t="n">
+        <v>0</v>
+      </c>
+      <c r="H12" t="n">
+        <v>0.17</v>
+      </c>
+      <c r="I12" t="n">
+        <v>0.018</v>
+      </c>
+      <c r="J12" t="n">
+        <v>1.16</v>
+      </c>
+      <c r="K12" t="n">
+        <v>0.123</v>
+      </c>
+      <c r="L12" t="n">
+        <v>0.6879999999999999</v>
+      </c>
+      <c r="M12" t="n">
+        <v>0.5629999999999999</v>
+      </c>
+      <c r="N12" t="n">
+        <v>0.679880928999584</v>
+      </c>
+      <c r="O12" t="n">
+        <v>0.6379835743388964</v>
+      </c>
+      <c r="P12" t="n">
+        <v>0.5633764173008923</v>
+      </c>
+      <c r="Q12" t="n">
+        <v>0.554285014141064</v>
+      </c>
+      <c r="R12" t="n">
+        <v>0.6</v>
+      </c>
+      <c r="S12" t="n">
+        <v>0.5176470588235293</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="n">
+        <v>13</v>
+      </c>
+      <c r="B13" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="C13" t="n">
+        <v>0</v>
+      </c>
+      <c r="D13" t="n">
+        <v>0</v>
+      </c>
+      <c r="E13" t="n">
+        <v>0</v>
+      </c>
+      <c r="F13" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="G13" t="n">
+        <v>0</v>
+      </c>
+      <c r="H13" t="n">
+        <v>0.14</v>
+      </c>
+      <c r="I13" t="n">
+        <v>0.011</v>
+      </c>
+      <c r="J13" t="n">
+        <v>1.09</v>
+      </c>
+      <c r="K13" t="n">
+        <v>0.107</v>
+      </c>
+      <c r="L13" t="n">
+        <v>0.7</v>
+      </c>
+      <c r="M13" t="n">
+        <v>0.575</v>
+      </c>
+      <c r="N13" t="n">
+        <v>0.5362935620555723</v>
+      </c>
+      <c r="O13" t="n">
+        <v>0.5111353654009368</v>
+      </c>
+      <c r="P13" t="n">
+        <v>0.4820248394552958</v>
+      </c>
+      <c r="Q13" t="n">
+        <v>0.3959672666196148</v>
+      </c>
+      <c r="R13" t="n">
+        <v>0.6399999999999999</v>
+      </c>
+      <c r="S13" t="n">
+        <v>0.552941176470588</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="n">
+        <v>14</v>
+      </c>
+      <c r="B14" t="n">
+        <v>0</v>
+      </c>
+      <c r="C14" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="D14" t="n">
+        <v>0</v>
+      </c>
+      <c r="E14" t="n">
+        <v>0</v>
+      </c>
+      <c r="F14" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="G14" t="n">
+        <v>0</v>
+      </c>
+      <c r="H14" t="n">
+        <v>0.123</v>
+      </c>
+      <c r="I14" t="n">
+        <v>0.008</v>
+      </c>
+      <c r="J14" t="n">
+        <v>1.01</v>
+      </c>
+      <c r="K14" t="n">
+        <v>0.08799999999999999</v>
+      </c>
+      <c r="L14" t="n">
+        <v>0.65</v>
+      </c>
+      <c r="M14" t="n">
+        <v>0.663</v>
+      </c>
+      <c r="N14" t="n">
+        <v>0.4557583139215232</v>
+      </c>
+      <c r="O14" t="n">
+        <v>0.4433580795480286</v>
+      </c>
+      <c r="P14" t="n">
+        <v>0.3995693672476422</v>
+      </c>
+      <c r="Q14" t="n">
+        <v>0.2177688583849585</v>
+      </c>
+      <c r="R14" t="n">
+        <v>0.4800000000000001</v>
+      </c>
+      <c r="S14" t="n">
+        <v>0.8</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="n">
+        <v>15</v>
+      </c>
+      <c r="B15" t="n">
+        <v>0</v>
+      </c>
+      <c r="C15" t="n">
+        <v>0</v>
+      </c>
+      <c r="D15" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="E15" t="n">
+        <v>0</v>
+      </c>
+      <c r="F15" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="G15" t="n">
+        <v>0</v>
+      </c>
+      <c r="H15" t="n">
+        <v>0.145</v>
+      </c>
+      <c r="I15" t="n">
+        <v>0.013</v>
+      </c>
+      <c r="J15" t="n">
+        <v>1.07</v>
+      </c>
+      <c r="K15" t="n">
+        <v>0.103</v>
+      </c>
+      <c r="L15" t="n">
+        <v>0.7</v>
+      </c>
+      <c r="M15" t="n">
+        <v>0.5629999999999999</v>
+      </c>
+      <c r="N15" t="n">
+        <v>0.561434189363648</v>
+      </c>
+      <c r="O15" t="n">
+        <v>0.5392707647759417</v>
+      </c>
+      <c r="P15" t="n">
+        <v>0.458220227639869</v>
+      </c>
+      <c r="Q15" t="n">
+        <v>0.3639989914705289</v>
+      </c>
+      <c r="R15" t="n">
+        <v>0.6399999999999999</v>
+      </c>
+      <c r="S15" t="n">
+        <v>0.5176470588235293</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="n">
+        <v>16</v>
+      </c>
+      <c r="B16" t="n">
+        <v>0</v>
+      </c>
+      <c r="C16" t="n">
+        <v>0</v>
+      </c>
+      <c r="D16" t="n">
+        <v>0</v>
+      </c>
+      <c r="E16" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="F16" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="G16" t="n">
+        <v>0</v>
+      </c>
+      <c r="H16" t="n">
+        <v>0.09</v>
+      </c>
+      <c r="I16" t="n">
+        <v>-0.001</v>
+      </c>
+      <c r="J16" t="n">
+        <v>1.15</v>
+      </c>
+      <c r="K16" t="n">
+        <v>0.109</v>
+      </c>
+      <c r="L16" t="n">
+        <v>0.663</v>
+      </c>
+      <c r="M16" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="N16" t="n">
+        <v>0.2982760574218143</v>
+      </c>
+      <c r="O16" t="n">
+        <v>0.2657154159440483</v>
+      </c>
+      <c r="P16" t="n">
+        <v>0.5496840704049175</v>
+      </c>
+      <c r="Q16" t="n">
+        <v>0.4152400963495619</v>
+      </c>
+      <c r="R16" t="n">
+        <v>0.5199999999999999</v>
+      </c>
+      <c r="S16" t="n">
+        <v>0.3411764705882353</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="n">
+        <v>17</v>
+      </c>
+      <c r="B17" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="C17" t="n">
+        <v>0</v>
+      </c>
+      <c r="D17" t="n">
+        <v>0</v>
+      </c>
+      <c r="E17" t="n">
+        <v>0</v>
+      </c>
+      <c r="F17" t="n">
+        <v>0</v>
+      </c>
+      <c r="G17" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="H17" t="n">
+        <v>0.118</v>
+      </c>
+      <c r="I17" t="n">
+        <v>0.008999999999999999</v>
+      </c>
+      <c r="J17" t="n">
+        <v>0.97</v>
+      </c>
+      <c r="K17" t="n">
+        <v>0.109</v>
+      </c>
+      <c r="L17" t="n">
+        <v>0.6879999999999999</v>
+      </c>
+      <c r="M17" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="N17" t="n">
+        <v>0.42967704121827</v>
+      </c>
+      <c r="O17" t="n">
+        <v>0.4741056620390809</v>
+      </c>
+      <c r="P17" t="n">
+        <v>0.3569834788339457</v>
+      </c>
+      <c r="Q17" t="n">
+        <v>0.4159127558769511</v>
+      </c>
+      <c r="R17" t="n">
+        <v>0.6</v>
+      </c>
+      <c r="S17" t="n">
+        <v>0.3411764705882353</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="n">
+        <v>18</v>
+      </c>
+      <c r="B18" t="n">
+        <v>0</v>
+      </c>
+      <c r="C18" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="D18" t="n">
+        <v>0</v>
+      </c>
+      <c r="E18" t="n">
+        <v>0</v>
+      </c>
+      <c r="F18" t="n">
+        <v>0</v>
+      </c>
+      <c r="G18" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="H18" t="n">
+        <v>0.154</v>
+      </c>
+      <c r="I18" t="n">
+        <v>0.017</v>
+      </c>
+      <c r="J18" t="n">
+        <v>0.99</v>
+      </c>
+      <c r="K18" t="n">
+        <v>0.101</v>
+      </c>
+      <c r="L18" t="n">
+        <v>0.675</v>
+      </c>
+      <c r="M18" t="n">
+        <v>0.625</v>
+      </c>
+      <c r="N18" t="n">
+        <v>0.6050396940893124</v>
+      </c>
+      <c r="O18" t="n">
+        <v>0.612416344592712</v>
+      </c>
+      <c r="P18" t="n">
+        <v>0.3741633884763284</v>
+      </c>
+      <c r="Q18" t="n">
+        <v>0.3438370551804509</v>
+      </c>
+      <c r="R18" t="n">
+        <v>0.5600000000000001</v>
+      </c>
+      <c r="S18" t="n">
+        <v>0.6941176470588235</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="n">
+        <v>19</v>
+      </c>
+      <c r="B19" t="n">
+        <v>0</v>
+      </c>
+      <c r="C19" t="n">
+        <v>0</v>
+      </c>
+      <c r="D19" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="E19" t="n">
+        <v>0</v>
+      </c>
+      <c r="F19" t="n">
+        <v>0</v>
+      </c>
+      <c r="G19" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="H19" t="n">
+        <v>0.138</v>
+      </c>
+      <c r="I19" t="n">
+        <v>0.013</v>
+      </c>
+      <c r="J19" t="n">
+        <v>1.04</v>
+      </c>
+      <c r="K19" t="n">
+        <v>0.114</v>
+      </c>
+      <c r="L19" t="n">
+        <v>0.638</v>
+      </c>
+      <c r="M19" t="n">
+        <v>0.55</v>
+      </c>
+      <c r="N19" t="n">
+        <v>0.5269834737017153</v>
+      </c>
+      <c r="O19" t="n">
+        <v>0.5435749708098773</v>
+      </c>
+      <c r="P19" t="n">
+        <v>0.4264384891027438</v>
+      </c>
+      <c r="Q19" t="n">
+        <v>0.4616038722163514</v>
+      </c>
+      <c r="R19" t="n">
+        <v>0.4399999999999998</v>
+      </c>
+      <c r="S19" t="n">
+        <v>0.4823529411764707</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="n">
+        <v>20</v>
+      </c>
+      <c r="B20" t="n">
+        <v>0</v>
+      </c>
+      <c r="C20" t="n">
+        <v>0</v>
+      </c>
+      <c r="D20" t="n">
+        <v>0</v>
+      </c>
+      <c r="E20" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="F20" t="n">
+        <v>0</v>
+      </c>
+      <c r="G20" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="H20" t="n">
+        <v>0.101</v>
+      </c>
+      <c r="I20" t="n">
+        <v>0.003</v>
+      </c>
+      <c r="J20" t="n">
+        <v>1.12</v>
+      </c>
+      <c r="K20" t="n">
+        <v>0.122</v>
+      </c>
+      <c r="L20" t="n">
+        <v>0.613</v>
+      </c>
+      <c r="M20" t="n">
+        <v>0.488</v>
+      </c>
+      <c r="N20" t="n">
+        <v>0.3494578554594443</v>
+      </c>
+      <c r="O20" t="n">
+        <v>0.3555004331214481</v>
+      </c>
+      <c r="P20" t="n">
+        <v>0.5149819362738174</v>
+      </c>
+      <c r="Q20" t="n">
+        <v>0.5371847315073373</v>
+      </c>
+      <c r="R20" t="n">
+        <v>0.3600000000000001</v>
+      </c>
+      <c r="S20" t="n">
+        <v>0.3058823529411764</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="n">
+        <v>21</v>
+      </c>
+      <c r="B21" t="n">
+        <v>0</v>
+      </c>
+      <c r="C21" t="n">
+        <v>0</v>
+      </c>
+      <c r="D21" t="n">
+        <v>0</v>
+      </c>
+      <c r="E21" t="n">
+        <v>0</v>
+      </c>
+      <c r="F21" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="G21" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="H21" t="n">
+        <v>0.093</v>
+      </c>
+      <c r="I21" t="n">
+        <v>0.001</v>
+      </c>
+      <c r="J21" t="n">
+        <v>1.01</v>
+      </c>
+      <c r="K21" t="n">
+        <v>0.091</v>
+      </c>
+      <c r="L21" t="n">
+        <v>0.625</v>
+      </c>
+      <c r="M21" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="N21" t="n">
+        <v>0.3122452028413787</v>
+      </c>
+      <c r="O21" t="n">
+        <v>0.3103632450658586</v>
+      </c>
+      <c r="P21" t="n">
+        <v>0.4034175600270007</v>
+      </c>
+      <c r="Q21" t="n">
+        <v>0.2404732341716849</v>
+      </c>
+      <c r="R21" t="n">
+        <v>0.4</v>
+      </c>
+      <c r="S21" t="n">
+        <v>0.3411764705882353</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="n">
+        <v>22</v>
+      </c>
+      <c r="B22" t="n">
+        <v>0.333</v>
+      </c>
+      <c r="C22" t="n">
+        <v>0.333</v>
+      </c>
+      <c r="D22" t="n">
+        <v>0.333</v>
+      </c>
+      <c r="E22" t="n">
+        <v>0</v>
+      </c>
+      <c r="F22" t="n">
+        <v>0</v>
+      </c>
+      <c r="G22" t="n">
+        <v>0</v>
+      </c>
+      <c r="H22" t="n">
+        <v>0.192</v>
+      </c>
+      <c r="I22" t="n">
+        <v>0.024</v>
+      </c>
+      <c r="J22" t="n">
+        <v>1.08</v>
+      </c>
+      <c r="K22" t="n">
+        <v>0.117</v>
+      </c>
+      <c r="L22" t="n">
+        <v>0.7</v>
+      </c>
+      <c r="M22" t="n">
+        <v>0.65</v>
+      </c>
+      <c r="N22" t="n">
+        <v>0.7860636531205283</v>
+      </c>
+      <c r="O22" t="n">
+        <v>0.7603576740349607</v>
+      </c>
+      <c r="P22" t="n">
+        <v>0.4721364107361539</v>
+      </c>
+      <c r="Q22" t="n">
+        <v>0.4917616365744848</v>
+      </c>
+      <c r="R22" t="n">
+        <v>0.6399999999999999</v>
+      </c>
+      <c r="S22" t="n">
+        <v>0.7647058823529413</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="n">
+        <v>23</v>
+      </c>
+      <c r="B23" t="n">
+        <v>0.333</v>
+      </c>
+      <c r="C23" t="n">
+        <v>0.333</v>
+      </c>
+      <c r="D23" t="n">
+        <v>0</v>
+      </c>
+      <c r="E23" t="n">
+        <v>0.333</v>
+      </c>
+      <c r="F23" t="n">
+        <v>0</v>
+      </c>
+      <c r="G23" t="n">
+        <v>0</v>
+      </c>
+      <c r="H23" t="n">
+        <v>0.183</v>
+      </c>
+      <c r="I23" t="n">
+        <v>0.023</v>
+      </c>
+      <c r="J23" t="n">
+        <v>0.98</v>
+      </c>
+      <c r="K23" t="n">
+        <v>0.102</v>
+      </c>
+      <c r="L23" t="n">
+        <v>0.725</v>
+      </c>
+      <c r="M23" t="n">
+        <v>0.575</v>
+      </c>
+      <c r="N23" t="n">
+        <v>0.7401201495879017</v>
+      </c>
+      <c r="O23" t="n">
+        <v>0.7394762683740155</v>
+      </c>
+      <c r="P23" t="n">
+        <v>0.3654027377743194</v>
+      </c>
+      <c r="Q23" t="n">
+        <v>0.3546558020456409</v>
+      </c>
+      <c r="R23" t="n">
+        <v>0.72</v>
+      </c>
+      <c r="S23" t="n">
+        <v>0.552941176470588</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="n">
+        <v>24</v>
+      </c>
+      <c r="B24" t="n">
+        <v>0.333</v>
+      </c>
+      <c r="C24" t="n">
+        <v>0</v>
+      </c>
+      <c r="D24" t="n">
+        <v>0.333</v>
+      </c>
+      <c r="E24" t="n">
+        <v>0.333</v>
+      </c>
+      <c r="F24" t="n">
+        <v>0</v>
+      </c>
+      <c r="G24" t="n">
+        <v>0</v>
+      </c>
+      <c r="H24" t="n">
+        <v>0.164</v>
+      </c>
+      <c r="I24" t="n">
+        <v>0.017</v>
+      </c>
+      <c r="J24" t="n">
+        <v>1.14</v>
+      </c>
+      <c r="K24" t="n">
+        <v>0.124</v>
+      </c>
+      <c r="L24" t="n">
+        <v>0.7</v>
+      </c>
+      <c r="M24" t="n">
+        <v>0.488</v>
+      </c>
+      <c r="N24" t="n">
+        <v>0.6517287495466886</v>
+      </c>
+      <c r="O24" t="n">
+        <v>0.6252758714415705</v>
+      </c>
+      <c r="P24" t="n">
+        <v>0.5346500091191823</v>
+      </c>
+      <c r="Q24" t="n">
+        <v>0.5617110796663136</v>
+      </c>
+      <c r="R24" t="n">
+        <v>0.6399999999999999</v>
+      </c>
+      <c r="S24" t="n">
+        <v>0.3058823529411764</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="n">
+        <v>25</v>
+      </c>
+      <c r="B25" t="n">
+        <v>0</v>
+      </c>
+      <c r="C25" t="n">
+        <v>0.333</v>
+      </c>
+      <c r="D25" t="n">
+        <v>0.333</v>
+      </c>
+      <c r="E25" t="n">
+        <v>0.333</v>
+      </c>
+      <c r="F25" t="n">
+        <v>0</v>
+      </c>
+      <c r="G25" t="n">
+        <v>0</v>
+      </c>
+      <c r="H25" t="n">
+        <v>0.184</v>
+      </c>
+      <c r="I25" t="n">
+        <v>0.022</v>
+      </c>
+      <c r="J25" t="n">
+        <v>1.07</v>
+      </c>
+      <c r="K25" t="n">
+        <v>0.109</v>
+      </c>
+      <c r="L25" t="n">
+        <v>0.7</v>
+      </c>
+      <c r="M25" t="n">
+        <v>0.613</v>
+      </c>
+      <c r="N25" t="n">
+        <v>0.7469285771240153</v>
+      </c>
+      <c r="O25" t="n">
+        <v>0.712062507446185</v>
+      </c>
+      <c r="P25" t="n">
+        <v>0.4670691747336297</v>
+      </c>
+      <c r="Q25" t="n">
+        <v>0.4141181687925621</v>
+      </c>
+      <c r="R25" t="n">
+        <v>0.6399999999999999</v>
+      </c>
+      <c r="S25" t="n">
+        <v>0.6588235294117648</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="n">
+        <v>26</v>
+      </c>
+      <c r="B26" t="n">
+        <v>0.333</v>
+      </c>
+      <c r="C26" t="n">
+        <v>0.333</v>
+      </c>
+      <c r="D26" t="n">
+        <v>0</v>
+      </c>
+      <c r="E26" t="n">
+        <v>0</v>
+      </c>
+      <c r="F26" t="n">
+        <v>0.333</v>
+      </c>
+      <c r="G26" t="n">
+        <v>0</v>
+      </c>
+      <c r="H26" t="n">
+        <v>0.147</v>
+      </c>
+      <c r="I26" t="n">
+        <v>0.015</v>
+      </c>
+      <c r="J26" t="n">
+        <v>0.95</v>
+      </c>
+      <c r="K26" t="n">
+        <v>0.092</v>
+      </c>
+      <c r="L26" t="n">
+        <v>0.713</v>
+      </c>
+      <c r="M26" t="n">
+        <v>0.625</v>
+      </c>
+      <c r="N26" t="n">
+        <v>0.5698583438629288</v>
+      </c>
+      <c r="O26" t="n">
+        <v>0.58074117908942</v>
+      </c>
+      <c r="P26" t="n">
+        <v>0.3397598984642516</v>
+      </c>
+      <c r="Q26" t="n">
+        <v>0.2524676057023322</v>
+      </c>
+      <c r="R26" t="n">
+        <v>0.6800000000000002</v>
+      </c>
+      <c r="S26" t="n">
+        <v>0.6941176470588235</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="n">
+        <v>27</v>
+      </c>
+      <c r="B27" t="n">
+        <v>0.333</v>
+      </c>
+      <c r="C27" t="n">
+        <v>0</v>
+      </c>
+      <c r="D27" t="n">
+        <v>0.333</v>
+      </c>
+      <c r="E27" t="n">
+        <v>0</v>
+      </c>
+      <c r="F27" t="n">
+        <v>0.333</v>
+      </c>
+      <c r="G27" t="n">
+        <v>0</v>
+      </c>
+      <c r="H27" t="n">
+        <v>0.168</v>
+      </c>
+      <c r="I27" t="n">
+        <v>0.017</v>
+      </c>
+      <c r="J27" t="n">
+        <v>1.17</v>
+      </c>
+      <c r="K27" t="n">
+        <v>0.122</v>
+      </c>
+      <c r="L27" t="n">
+        <v>0.675</v>
+      </c>
+      <c r="M27" t="n">
+        <v>0.588</v>
+      </c>
+      <c r="N27" t="n">
+        <v>0.6675812496113429</v>
+      </c>
+      <c r="O27" t="n">
+        <v>0.6205260413415092</v>
+      </c>
+      <c r="P27" t="n">
+        <v>0.5650982059480344</v>
+      </c>
+      <c r="Q27" t="n">
+        <v>0.5428003842435933</v>
+      </c>
+      <c r="R27" t="n">
+        <v>0.5600000000000001</v>
+      </c>
+      <c r="S27" t="n">
+        <v>0.5882352941176472</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="n">
+        <v>28</v>
+      </c>
+      <c r="B28" t="n">
+        <v>0</v>
+      </c>
+      <c r="C28" t="n">
+        <v>0.333</v>
+      </c>
+      <c r="D28" t="n">
+        <v>0.333</v>
+      </c>
+      <c r="E28" t="n">
+        <v>0</v>
+      </c>
+      <c r="F28" t="n">
+        <v>0.333</v>
+      </c>
+      <c r="G28" t="n">
+        <v>0</v>
+      </c>
+      <c r="H28" t="n">
+        <v>0.146</v>
+      </c>
+      <c r="I28" t="n">
+        <v>0.014</v>
+      </c>
+      <c r="J28" t="n">
+        <v>0.99</v>
+      </c>
+      <c r="K28" t="n">
+        <v>0.093</v>
+      </c>
+      <c r="L28" t="n">
+        <v>0.675</v>
+      </c>
+      <c r="M28" t="n">
+        <v>0.6</v>
+      </c>
+      <c r="N28" t="n">
+        <v>0.5666519339926036</v>
+      </c>
+      <c r="O28" t="n">
+        <v>0.5622273810347056</v>
+      </c>
+      <c r="P28" t="n">
+        <v>0.3787264276314638</v>
+      </c>
+      <c r="Q28" t="n">
+        <v>0.2673011504813086</v>
+      </c>
+      <c r="R28" t="n">
+        <v>0.5600000000000001</v>
+      </c>
+      <c r="S28" t="n">
+        <v>0.6235294117647059</v>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="n">
+        <v>29</v>
+      </c>
+      <c r="B29" t="n">
+        <v>0.333</v>
+      </c>
+      <c r="C29" t="n">
+        <v>0</v>
+      </c>
+      <c r="D29" t="n">
+        <v>0</v>
+      </c>
+      <c r="E29" t="n">
+        <v>0.333</v>
+      </c>
+      <c r="F29" t="n">
+        <v>0.333</v>
+      </c>
+      <c r="G29" t="n">
+        <v>0</v>
+      </c>
+      <c r="H29" t="n">
+        <v>0.127</v>
+      </c>
+      <c r="I29" t="n">
+        <v>0.01</v>
+      </c>
+      <c r="J29" t="n">
+        <v>0.99</v>
+      </c>
+      <c r="K29" t="n">
+        <v>0.096</v>
+      </c>
+      <c r="L29" t="n">
+        <v>0.6879999999999999</v>
+      </c>
+      <c r="M29" t="n">
+        <v>0.538</v>
+      </c>
+      <c r="N29" t="n">
+        <v>0.4739678490113821</v>
+      </c>
+      <c r="O29" t="n">
+        <v>0.4824636708697147</v>
+      </c>
+      <c r="P29" t="n">
+        <v>0.3754391038884727</v>
+      </c>
+      <c r="Q29" t="n">
+        <v>0.2933121985773124</v>
+      </c>
+      <c r="R29" t="n">
+        <v>0.6</v>
+      </c>
+      <c r="S29" t="n">
+        <v>0.4470588235294117</v>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="n">
+        <v>30</v>
+      </c>
+      <c r="B30" t="n">
+        <v>0</v>
+      </c>
+      <c r="C30" t="n">
+        <v>0.333</v>
+      </c>
+      <c r="D30" t="n">
+        <v>0</v>
+      </c>
+      <c r="E30" t="n">
+        <v>0.333</v>
+      </c>
+      <c r="F30" t="n">
+        <v>0.333</v>
+      </c>
+      <c r="G30" t="n">
+        <v>0</v>
+      </c>
+      <c r="H30" t="n">
+        <v>0.124</v>
+      </c>
+      <c r="I30" t="n">
+        <v>0.007</v>
+      </c>
+      <c r="J30" t="n">
+        <v>1.09</v>
+      </c>
+      <c r="K30" t="n">
+        <v>0.101</v>
+      </c>
+      <c r="L30" t="n">
+        <v>0.675</v>
+      </c>
+      <c r="M30" t="n">
+        <v>0.588</v>
+      </c>
+      <c r="N30" t="n">
+        <v>0.4611824703977668</v>
+      </c>
+      <c r="O30" t="n">
+        <v>0.429774097719644</v>
+      </c>
+      <c r="P30" t="n">
+        <v>0.4859414322090453</v>
+      </c>
+      <c r="Q30" t="n">
+        <v>0.3371043929867878</v>
+      </c>
+      <c r="R30" t="n">
+        <v>0.5600000000000001</v>
+      </c>
+      <c r="S30" t="n">
+        <v>0.5882352941176472</v>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="n">
+        <v>31</v>
+      </c>
+      <c r="B31" t="n">
+        <v>0</v>
+      </c>
+      <c r="C31" t="n">
+        <v>0</v>
+      </c>
+      <c r="D31" t="n">
+        <v>0.333</v>
+      </c>
+      <c r="E31" t="n">
+        <v>0.333</v>
+      </c>
+      <c r="F31" t="n">
+        <v>0.333</v>
+      </c>
+      <c r="G31" t="n">
+        <v>0</v>
+      </c>
+      <c r="H31" t="n">
+        <v>0.138</v>
+      </c>
+      <c r="I31" t="n">
+        <v>0.012</v>
+      </c>
+      <c r="J31" t="n">
+        <v>1.04</v>
+      </c>
+      <c r="K31" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="L31" t="n">
+        <v>0.675</v>
+      </c>
+      <c r="M31" t="n">
+        <v>0.6</v>
+      </c>
+      <c r="N31" t="n">
+        <v>0.5267339839954777</v>
+      </c>
+      <c r="O31" t="n">
+        <v>0.5141391142226678</v>
+      </c>
+      <c r="P31" t="n">
+        <v>0.430226316596444</v>
+      </c>
+      <c r="Q31" t="n">
+        <v>0.3352125099642292</v>
+      </c>
+      <c r="R31" t="n">
+        <v>0.5600000000000001</v>
+      </c>
+      <c r="S31" t="n">
+        <v>0.6235294117647059</v>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="n">
+        <v>32</v>
+      </c>
+      <c r="B32" t="n">
+        <v>0.333</v>
+      </c>
+      <c r="C32" t="n">
+        <v>0.333</v>
+      </c>
+      <c r="D32" t="n">
+        <v>0</v>
+      </c>
+      <c r="E32" t="n">
+        <v>0</v>
+      </c>
+      <c r="F32" t="n">
+        <v>0</v>
+      </c>
+      <c r="G32" t="n">
+        <v>0.333</v>
+      </c>
+      <c r="H32" t="n">
+        <v>0.17</v>
+      </c>
+      <c r="I32" t="n">
+        <v>0.024</v>
+      </c>
+      <c r="J32" t="n">
+        <v>0.82</v>
+      </c>
+      <c r="K32" t="n">
+        <v>0.094</v>
+      </c>
+      <c r="L32" t="n">
+        <v>0.738</v>
+      </c>
+      <c r="M32" t="n">
+        <v>0.5629999999999999</v>
+      </c>
+      <c r="N32" t="n">
+        <v>0.678478990474893</v>
+      </c>
+      <c r="O32" t="n">
+        <v>0.7459957522066218</v>
+      </c>
+      <c r="P32" t="n">
+        <v>0.2</v>
+      </c>
+      <c r="Q32" t="n">
+        <v>0.276483388231805</v>
+      </c>
+      <c r="R32" t="n">
+        <v>0.7600000000000002</v>
+      </c>
+      <c r="S32" t="n">
+        <v>0.5176470588235293</v>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" t="n">
+        <v>33</v>
+      </c>
+      <c r="B33" t="n">
+        <v>0.333</v>
+      </c>
+      <c r="C33" t="n">
+        <v>0</v>
+      </c>
+      <c r="D33" t="n">
+        <v>0.333</v>
+      </c>
+      <c r="E33" t="n">
+        <v>0</v>
+      </c>
+      <c r="F33" t="n">
+        <v>0</v>
+      </c>
+      <c r="G33" t="n">
+        <v>0.333</v>
+      </c>
+      <c r="H33" t="n">
+        <v>0.135</v>
+      </c>
+      <c r="I33" t="n">
+        <v>0.012</v>
+      </c>
+      <c r="J33" t="n">
+        <v>1.07</v>
+      </c>
+      <c r="K33" t="n">
+        <v>0.119</v>
+      </c>
+      <c r="L33" t="n">
+        <v>0.638</v>
+      </c>
+      <c r="M33" t="n">
+        <v>0.525</v>
+      </c>
+      <c r="N33" t="n">
+        <v>0.5126785677832426</v>
+      </c>
+      <c r="O33" t="n">
+        <v>0.5254941010226786</v>
+      </c>
+      <c r="P33" t="n">
+        <v>0.4595436786214912</v>
+      </c>
+      <c r="Q33" t="n">
+        <v>0.5105882451427618</v>
+      </c>
+      <c r="R33" t="n">
+        <v>0.4399999999999998</v>
+      </c>
+      <c r="S33" t="n">
+        <v>0.411764705882353</v>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" t="n">
+        <v>34</v>
+      </c>
+      <c r="B34" t="n">
+        <v>0</v>
+      </c>
+      <c r="C34" t="n">
+        <v>0.333</v>
+      </c>
+      <c r="D34" t="n">
+        <v>0.333</v>
+      </c>
+      <c r="E34" t="n">
+        <v>0</v>
+      </c>
+      <c r="F34" t="n">
+        <v>0</v>
+      </c>
+      <c r="G34" t="n">
+        <v>0.333</v>
+      </c>
+      <c r="H34" t="n">
+        <v>0.185</v>
+      </c>
+      <c r="I34" t="n">
+        <v>0.024</v>
+      </c>
+      <c r="J34" t="n">
+        <v>0.98</v>
+      </c>
+      <c r="K34" t="n">
+        <v>0.105</v>
+      </c>
+      <c r="L34" t="n">
+        <v>0.675</v>
+      </c>
+      <c r="M34" t="n">
+        <v>0.588</v>
+      </c>
+      <c r="N34" t="n">
+        <v>0.7534382783370357</v>
+      </c>
+      <c r="O34" t="n">
+        <v>0.7547581353036255</v>
+      </c>
+      <c r="P34" t="n">
+        <v>0.3685756589872907</v>
+      </c>
+      <c r="Q34" t="n">
+        <v>0.3772675777035235</v>
+      </c>
+      <c r="R34" t="n">
+        <v>0.5600000000000001</v>
+      </c>
+      <c r="S34" t="n">
+        <v>0.5882352941176472</v>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" t="n">
+        <v>35</v>
+      </c>
+      <c r="B35" t="n">
+        <v>0.333</v>
+      </c>
+      <c r="C35" t="n">
+        <v>0</v>
+      </c>
+      <c r="D35" t="n">
+        <v>0</v>
+      </c>
+      <c r="E35" t="n">
+        <v>0.333</v>
+      </c>
+      <c r="F35" t="n">
+        <v>0</v>
+      </c>
+      <c r="G35" t="n">
+        <v>0.333</v>
+      </c>
+      <c r="H35" t="n">
+        <v>0.127</v>
+      </c>
+      <c r="I35" t="n">
+        <v>0.011</v>
+      </c>
+      <c r="J35" t="n">
+        <v>0.9399999999999999</v>
+      </c>
+      <c r="K35" t="n">
+        <v>0.101</v>
+      </c>
+      <c r="L35" t="n">
+        <v>0.663</v>
+      </c>
+      <c r="M35" t="n">
+        <v>0.55</v>
+      </c>
+      <c r="N35" t="n">
+        <v>0.4712765239233735</v>
+      </c>
+      <c r="O35" t="n">
+        <v>0.5123513411762739</v>
+      </c>
+      <c r="P35" t="n">
+        <v>0.3251581359885314</v>
+      </c>
+      <c r="Q35" t="n">
+        <v>0.3387816881904299</v>
+      </c>
+      <c r="R35" t="n">
+        <v>0.5199999999999999</v>
+      </c>
+      <c r="S35" t="n">
+        <v>0.4823529411764707</v>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" t="n">
+        <v>36</v>
+      </c>
+      <c r="B36" t="n">
+        <v>0</v>
+      </c>
+      <c r="C36" t="n">
+        <v>0.333</v>
+      </c>
+      <c r="D36" t="n">
+        <v>0</v>
+      </c>
+      <c r="E36" t="n">
+        <v>0.333</v>
+      </c>
+      <c r="F36" t="n">
+        <v>0</v>
+      </c>
+      <c r="G36" t="n">
+        <v>0.333</v>
+      </c>
+      <c r="H36" t="n">
+        <v>0.156</v>
+      </c>
+      <c r="I36" t="n">
+        <v>0.017</v>
+      </c>
+      <c r="J36" t="n">
+        <v>0.99</v>
+      </c>
+      <c r="K36" t="n">
+        <v>0.103</v>
+      </c>
+      <c r="L36" t="n">
+        <v>0.65</v>
+      </c>
+      <c r="M36" t="n">
+        <v>0.575</v>
+      </c>
+      <c r="N36" t="n">
+        <v>0.6131639711976793</v>
+      </c>
+      <c r="O36" t="n">
+        <v>0.6213158908075199</v>
+      </c>
+      <c r="P36" t="n">
+        <v>0.3774650980183919</v>
+      </c>
+      <c r="Q36" t="n">
+        <v>0.356305217581819</v>
+      </c>
+      <c r="R36" t="n">
+        <v>0.4800000000000001</v>
+      </c>
+      <c r="S36" t="n">
+        <v>0.552941176470588</v>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" t="n">
+        <v>37</v>
+      </c>
+      <c r="B37" t="n">
+        <v>0</v>
+      </c>
+      <c r="C37" t="n">
+        <v>0</v>
+      </c>
+      <c r="D37" t="n">
+        <v>0.333</v>
+      </c>
+      <c r="E37" t="n">
+        <v>0.333</v>
+      </c>
+      <c r="F37" t="n">
+        <v>0</v>
+      </c>
+      <c r="G37" t="n">
+        <v>0.333</v>
+      </c>
+      <c r="H37" t="n">
+        <v>0.157</v>
+      </c>
+      <c r="I37" t="n">
+        <v>0.016</v>
+      </c>
+      <c r="J37" t="n">
+        <v>1.07</v>
+      </c>
+      <c r="K37" t="n">
+        <v>0.114</v>
+      </c>
+      <c r="L37" t="n">
+        <v>0.65</v>
+      </c>
+      <c r="M37" t="n">
+        <v>0.525</v>
+      </c>
+      <c r="N37" t="n">
+        <v>0.6186141276072736</v>
+      </c>
+      <c r="O37" t="n">
+        <v>0.6085807622816519</v>
+      </c>
+      <c r="P37" t="n">
+        <v>0.4653227151437824</v>
+      </c>
+      <c r="Q37" t="n">
+        <v>0.4643784259222708</v>
+      </c>
+      <c r="R37" t="n">
+        <v>0.4800000000000001</v>
+      </c>
+      <c r="S37" t="n">
+        <v>0.411764705882353</v>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" t="n">
+        <v>38</v>
+      </c>
+      <c r="B38" t="n">
+        <v>0.333</v>
+      </c>
+      <c r="C38" t="n">
+        <v>0</v>
+      </c>
+      <c r="D38" t="n">
+        <v>0</v>
+      </c>
+      <c r="E38" t="n">
+        <v>0</v>
+      </c>
+      <c r="F38" t="n">
+        <v>0.333</v>
+      </c>
+      <c r="G38" t="n">
+        <v>0.333</v>
+      </c>
+      <c r="H38" t="n">
+        <v>0.138</v>
+      </c>
+      <c r="I38" t="n">
+        <v>0.014</v>
+      </c>
+      <c r="J38" t="n">
+        <v>0.96</v>
+      </c>
+      <c r="K38" t="n">
+        <v>0.101</v>
+      </c>
+      <c r="L38" t="n">
+        <v>0.7</v>
+      </c>
+      <c r="M38" t="n">
+        <v>0.55</v>
+      </c>
+      <c r="N38" t="n">
+        <v>0.526337790334503</v>
+      </c>
+      <c r="O38" t="n">
+        <v>0.5522684092416684</v>
+      </c>
+      <c r="P38" t="n">
+        <v>0.3481275323032848</v>
+      </c>
+      <c r="Q38" t="n">
+        <v>0.3394951883837048</v>
+      </c>
+      <c r="R38" t="n">
+        <v>0.6399999999999999</v>
+      </c>
+      <c r="S38" t="n">
+        <v>0.4823529411764707</v>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" t="n">
+        <v>39</v>
+      </c>
+      <c r="B39" t="n">
+        <v>0</v>
+      </c>
+      <c r="C39" t="n">
+        <v>0.333</v>
+      </c>
+      <c r="D39" t="n">
+        <v>0</v>
+      </c>
+      <c r="E39" t="n">
+        <v>0</v>
+      </c>
+      <c r="F39" t="n">
+        <v>0.333</v>
+      </c>
+      <c r="G39" t="n">
+        <v>0.333</v>
+      </c>
+      <c r="H39" t="n">
+        <v>0.138</v>
+      </c>
+      <c r="I39" t="n">
+        <v>0.012</v>
+      </c>
+      <c r="J39" t="n">
+        <v>0.97</v>
+      </c>
+      <c r="K39" t="n">
+        <v>0.08799999999999999</v>
+      </c>
+      <c r="L39" t="n">
+        <v>0.638</v>
+      </c>
+      <c r="M39" t="n">
+        <v>0.625</v>
+      </c>
+      <c r="N39" t="n">
+        <v>0.5250184789531993</v>
+      </c>
+      <c r="O39" t="n">
+        <v>0.5240469988994729</v>
+      </c>
+      <c r="P39" t="n">
+        <v>0.3581055250960084</v>
+      </c>
+      <c r="Q39" t="n">
+        <v>0.2152551964457102</v>
+      </c>
+      <c r="R39" t="n">
+        <v>0.4399999999999998</v>
+      </c>
+      <c r="S39" t="n">
+        <v>0.6941176470588235</v>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" t="n">
+        <v>40</v>
+      </c>
+      <c r="B40" t="n">
+        <v>0</v>
+      </c>
+      <c r="C40" t="n">
+        <v>0</v>
+      </c>
+      <c r="D40" t="n">
+        <v>0.333</v>
+      </c>
+      <c r="E40" t="n">
+        <v>0</v>
+      </c>
+      <c r="F40" t="n">
+        <v>0.333</v>
+      </c>
+      <c r="G40" t="n">
+        <v>0.333</v>
+      </c>
+      <c r="H40" t="n">
+        <v>0.141</v>
+      </c>
+      <c r="I40" t="n">
+        <v>0.014</v>
+      </c>
+      <c r="J40" t="n">
+        <v>0.95</v>
+      </c>
+      <c r="K40" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="L40" t="n">
+        <v>0.663</v>
+      </c>
+      <c r="M40" t="n">
+        <v>0.525</v>
+      </c>
+      <c r="N40" t="n">
+        <v>0.5422370283457758</v>
+      </c>
+      <c r="O40" t="n">
+        <v>0.5704681862914787</v>
+      </c>
+      <c r="P40" t="n">
+        <v>0.3384120639398084</v>
+      </c>
+      <c r="Q40" t="n">
+        <v>0.3340808547169822</v>
+      </c>
+      <c r="R40" t="n">
+        <v>0.5199999999999999</v>
+      </c>
+      <c r="S40" t="n">
+        <v>0.411764705882353</v>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" t="n">
+        <v>41</v>
+      </c>
+      <c r="B41" t="n">
+        <v>0</v>
+      </c>
+      <c r="C41" t="n">
+        <v>0</v>
+      </c>
+      <c r="D41" t="n">
+        <v>0</v>
+      </c>
+      <c r="E41" t="n">
+        <v>0.333</v>
+      </c>
+      <c r="F41" t="n">
+        <v>0.333</v>
+      </c>
+      <c r="G41" t="n">
+        <v>0.333</v>
+      </c>
+      <c r="H41" t="n">
+        <v>0.09</v>
+      </c>
+      <c r="I41" t="n">
+        <v>0</v>
+      </c>
+      <c r="J41" t="n">
+        <v>1.13</v>
+      </c>
+      <c r="K41" t="n">
+        <v>0.113</v>
+      </c>
+      <c r="L41" t="n">
+        <v>0.588</v>
+      </c>
+      <c r="M41" t="n">
+        <v>0.45</v>
+      </c>
+      <c r="N41" t="n">
+        <v>0.2951241946536911</v>
+      </c>
+      <c r="O41" t="n">
+        <v>0.2813027525823505</v>
+      </c>
+      <c r="P41" t="n">
+        <v>0.5249102131694026</v>
+      </c>
+      <c r="Q41" t="n">
+        <v>0.4582578057386329</v>
+      </c>
+      <c r="R41" t="n">
+        <v>0.2800000000000001</v>
+      </c>
+      <c r="S41" t="n">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" t="n">
+        <v>42</v>
+      </c>
+      <c r="B42" t="n">
+        <v>0.25</v>
+      </c>
+      <c r="C42" t="n">
+        <v>0.25</v>
+      </c>
+      <c r="D42" t="n">
+        <v>0.25</v>
+      </c>
+      <c r="E42" t="n">
+        <v>0.25</v>
+      </c>
+      <c r="F42" t="n">
+        <v>0</v>
+      </c>
+      <c r="G42" t="n">
+        <v>0</v>
+      </c>
+      <c r="H42" t="n">
+        <v>0.191</v>
+      </c>
+      <c r="I42" t="n">
+        <v>0.024</v>
+      </c>
+      <c r="J42" t="n">
+        <v>1.06</v>
+      </c>
+      <c r="K42" t="n">
+        <v>0.113</v>
+      </c>
+      <c r="L42" t="n">
+        <v>0.7</v>
+      </c>
+      <c r="M42" t="n">
+        <v>0.575</v>
+      </c>
+      <c r="N42" t="n">
+        <v>0.7804181771935204</v>
+      </c>
+      <c r="O42" t="n">
+        <v>0.7528343279604217</v>
+      </c>
+      <c r="P42" t="n">
+        <v>0.4568702407045757</v>
+      </c>
+      <c r="Q42" t="n">
+        <v>0.4572399548531218</v>
+      </c>
+      <c r="R42" t="n">
+        <v>0.6399999999999999</v>
+      </c>
+      <c r="S42" t="n">
+        <v>0.552941176470588</v>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" t="n">
+        <v>43</v>
+      </c>
+      <c r="B43" t="n">
+        <v>0.25</v>
+      </c>
+      <c r="C43" t="n">
+        <v>0.25</v>
+      </c>
+      <c r="D43" t="n">
+        <v>0.25</v>
+      </c>
+      <c r="E43" t="n">
+        <v>0</v>
+      </c>
+      <c r="F43" t="n">
+        <v>0.25</v>
+      </c>
+      <c r="G43" t="n">
+        <v>0</v>
+      </c>
+      <c r="H43" t="n">
+        <v>0.17</v>
+      </c>
+      <c r="I43" t="n">
+        <v>0.019</v>
+      </c>
+      <c r="J43" t="n">
+        <v>1.02</v>
+      </c>
+      <c r="K43" t="n">
+        <v>0.103</v>
+      </c>
+      <c r="L43" t="n">
+        <v>0.713</v>
+      </c>
+      <c r="M43" t="n">
+        <v>0.65</v>
+      </c>
+      <c r="N43" t="n">
+        <v>0.6793906898304591</v>
+      </c>
+      <c r="O43" t="n">
+        <v>0.6650283010880643</v>
+      </c>
+      <c r="P43" t="n">
+        <v>0.4145620331302436</v>
+      </c>
+      <c r="Q43" t="n">
+        <v>0.3627255020756905</v>
+      </c>
+      <c r="R43" t="n">
+        <v>0.6800000000000002</v>
+      </c>
+      <c r="S43" t="n">
+        <v>0.7647058823529413</v>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" t="n">
+        <v>44</v>
+      </c>
+      <c r="B44" t="n">
+        <v>0.25</v>
+      </c>
+      <c r="C44" t="n">
+        <v>0.25</v>
+      </c>
+      <c r="D44" t="n">
+        <v>0</v>
+      </c>
+      <c r="E44" t="n">
+        <v>0.25</v>
+      </c>
+      <c r="F44" t="n">
+        <v>0.25</v>
+      </c>
+      <c r="G44" t="n">
+        <v>0</v>
+      </c>
+      <c r="H44" t="n">
+        <v>0.15</v>
+      </c>
+      <c r="I44" t="n">
+        <v>0.015</v>
+      </c>
+      <c r="J44" t="n">
+        <v>0.98</v>
+      </c>
+      <c r="K44" t="n">
+        <v>0.093</v>
+      </c>
+      <c r="L44" t="n">
+        <v>0.7</v>
+      </c>
+      <c r="M44" t="n">
+        <v>0.613</v>
+      </c>
+      <c r="N44" t="n">
+        <v>0.5823572588568386</v>
+      </c>
+      <c r="O44" t="n">
+        <v>0.5816009817634683</v>
+      </c>
+      <c r="P44" t="n">
+        <v>0.3651775768235799</v>
+      </c>
+      <c r="Q44" t="n">
+        <v>0.2634732849941864</v>
+      </c>
+      <c r="R44" t="n">
+        <v>0.6399999999999999</v>
+      </c>
+      <c r="S44" t="n">
+        <v>0.6588235294117648</v>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" t="n">
+        <v>45</v>
+      </c>
+      <c r="B45" t="n">
+        <v>0.25</v>
+      </c>
+      <c r="C45" t="n">
+        <v>0</v>
+      </c>
+      <c r="D45" t="n">
+        <v>0.25</v>
+      </c>
+      <c r="E45" t="n">
+        <v>0.25</v>
+      </c>
+      <c r="F45" t="n">
+        <v>0.25</v>
+      </c>
+      <c r="G45" t="n">
+        <v>0</v>
+      </c>
+      <c r="H45" t="n">
+        <v>0.153</v>
+      </c>
+      <c r="I45" t="n">
+        <v>0.015</v>
+      </c>
+      <c r="J45" t="n">
+        <v>1.08</v>
+      </c>
+      <c r="K45" t="n">
+        <v>0.111</v>
+      </c>
+      <c r="L45" t="n">
+        <v>0.663</v>
+      </c>
+      <c r="M45" t="n">
+        <v>0.538</v>
+      </c>
+      <c r="N45" t="n">
+        <v>0.5985157652025039</v>
+      </c>
+      <c r="O45" t="n">
+        <v>0.5804378784638089</v>
+      </c>
+      <c r="P45" t="n">
+        <v>0.4690062774254209</v>
+      </c>
+      <c r="Q45" t="n">
+        <v>0.434922325529349</v>
+      </c>
+      <c r="R45" t="n">
+        <v>0.5199999999999999</v>
+      </c>
+      <c r="S45" t="n">
+        <v>0.4470588235294117</v>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" t="n">
+        <v>46</v>
+      </c>
+      <c r="B46" t="n">
+        <v>0</v>
+      </c>
+      <c r="C46" t="n">
+        <v>0.25</v>
+      </c>
+      <c r="D46" t="n">
+        <v>0.25</v>
+      </c>
+      <c r="E46" t="n">
+        <v>0.25</v>
+      </c>
+      <c r="F46" t="n">
+        <v>0.25</v>
+      </c>
+      <c r="G46" t="n">
+        <v>0</v>
+      </c>
+      <c r="H46" t="n">
+        <v>0.152</v>
+      </c>
+      <c r="I46" t="n">
+        <v>0.014</v>
+      </c>
+      <c r="J46" t="n">
+        <v>1.05</v>
+      </c>
+      <c r="K46" t="n">
+        <v>0.098</v>
+      </c>
+      <c r="L46" t="n">
+        <v>0.675</v>
+      </c>
+      <c r="M46" t="n">
+        <v>0.625</v>
+      </c>
+      <c r="N46" t="n">
+        <v>0.595111073916493</v>
+      </c>
+      <c r="O46" t="n">
+        <v>0.5683591517019816</v>
+      </c>
+      <c r="P46" t="n">
+        <v>0.4404155271330232</v>
+      </c>
+      <c r="Q46" t="n">
+        <v>0.3153692944878067</v>
+      </c>
+      <c r="R46" t="n">
+        <v>0.5600000000000001</v>
+      </c>
+      <c r="S46" t="n">
+        <v>0.6941176470588235</v>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" t="n">
+        <v>47</v>
+      </c>
+      <c r="B47" t="n">
+        <v>0.25</v>
+      </c>
+      <c r="C47" t="n">
+        <v>0.25</v>
+      </c>
+      <c r="D47" t="n">
+        <v>0.25</v>
+      </c>
+      <c r="E47" t="n">
+        <v>0</v>
+      </c>
+      <c r="F47" t="n">
+        <v>0</v>
+      </c>
+      <c r="G47" t="n">
+        <v>0.25</v>
+      </c>
+      <c r="H47" t="n">
+        <v>0.177</v>
+      </c>
+      <c r="I47" t="n">
+        <v>0.023</v>
+      </c>
+      <c r="J47" t="n">
+        <v>0.97</v>
+      </c>
+      <c r="K47" t="n">
+        <v>0.108</v>
+      </c>
+      <c r="L47" t="n">
+        <v>0.6879999999999999</v>
+      </c>
+      <c r="M47" t="n">
+        <v>0.588</v>
+      </c>
+      <c r="N47" t="n">
+        <v>0.7136073235412168</v>
+      </c>
+      <c r="O47" t="n">
+        <v>0.7316166601888014</v>
+      </c>
+      <c r="P47" t="n">
+        <v>0.3577124284423606</v>
+      </c>
+      <c r="Q47" t="n">
+        <v>0.4120040139196675</v>
+      </c>
+      <c r="R47" t="n">
+        <v>0.6</v>
+      </c>
+      <c r="S47" t="n">
+        <v>0.5882352941176472</v>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" t="n">
+        <v>48</v>
+      </c>
+      <c r="B48" t="n">
+        <v>0.25</v>
+      </c>
+      <c r="C48" t="n">
+        <v>0.25</v>
+      </c>
+      <c r="D48" t="n">
+        <v>0</v>
+      </c>
+      <c r="E48" t="n">
+        <v>0.25</v>
+      </c>
+      <c r="F48" t="n">
+        <v>0</v>
+      </c>
+      <c r="G48" t="n">
+        <v>0.25</v>
+      </c>
+      <c r="H48" t="n">
+        <v>0.17</v>
+      </c>
+      <c r="I48" t="n">
+        <v>0.023</v>
+      </c>
+      <c r="J48" t="n">
+        <v>0.86</v>
+      </c>
+      <c r="K48" t="n">
+        <v>0.094</v>
+      </c>
+      <c r="L48" t="n">
+        <v>0.675</v>
+      </c>
+      <c r="M48" t="n">
+        <v>0.638</v>
+      </c>
+      <c r="N48" t="n">
+        <v>0.6808654615806808</v>
+      </c>
+      <c r="O48" t="n">
+        <v>0.7291441185815164</v>
+      </c>
+      <c r="P48" t="n">
+        <v>0.2394711949783647</v>
+      </c>
+      <c r="Q48" t="n">
+        <v>0.2703766065374231</v>
+      </c>
+      <c r="R48" t="n">
+        <v>0.5600000000000001</v>
+      </c>
+      <c r="S48" t="n">
+        <v>0.7294117647058822</v>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" t="n">
+        <v>49</v>
+      </c>
+      <c r="B49" t="n">
+        <v>0.25</v>
+      </c>
+      <c r="C49" t="n">
+        <v>0</v>
+      </c>
+      <c r="D49" t="n">
+        <v>0.25</v>
+      </c>
+      <c r="E49" t="n">
+        <v>0.25</v>
+      </c>
+      <c r="F49" t="n">
+        <v>0</v>
+      </c>
+      <c r="G49" t="n">
+        <v>0.25</v>
+      </c>
+      <c r="H49" t="n">
+        <v>0.154</v>
+      </c>
+      <c r="I49" t="n">
+        <v>0.017</v>
+      </c>
+      <c r="J49" t="n">
+        <v>1.04</v>
+      </c>
+      <c r="K49" t="n">
+        <v>0.117</v>
+      </c>
+      <c r="L49" t="n">
+        <v>0.65</v>
+      </c>
+      <c r="M49" t="n">
+        <v>0.513</v>
+      </c>
+      <c r="N49" t="n">
+        <v>0.600994857018337</v>
+      </c>
+      <c r="O49" t="n">
+        <v>0.6125773131041341</v>
+      </c>
+      <c r="P49" t="n">
+        <v>0.4320050484842241</v>
+      </c>
+      <c r="Q49" t="n">
+        <v>0.4924059557443084</v>
+      </c>
+      <c r="R49" t="n">
+        <v>0.4800000000000001</v>
+      </c>
+      <c r="S49" t="n">
+        <v>0.376470588235294</v>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50" t="n">
+        <v>50</v>
+      </c>
+      <c r="B50" t="n">
+        <v>0</v>
+      </c>
+      <c r="C50" t="n">
+        <v>0.25</v>
+      </c>
+      <c r="D50" t="n">
+        <v>0.25</v>
+      </c>
+      <c r="E50" t="n">
+        <v>0.25</v>
+      </c>
+      <c r="F50" t="n">
+        <v>0</v>
+      </c>
+      <c r="G50" t="n">
+        <v>0.25</v>
+      </c>
+      <c r="H50" t="n">
+        <v>0.179</v>
+      </c>
+      <c r="I50" t="n">
+        <v>0.022</v>
+      </c>
+      <c r="J50" t="n">
+        <v>1</v>
+      </c>
+      <c r="K50" t="n">
+        <v>0.106</v>
+      </c>
+      <c r="L50" t="n">
+        <v>0.713</v>
+      </c>
+      <c r="M50" t="n">
+        <v>0.613</v>
+      </c>
+      <c r="N50" t="n">
+        <v>0.721101908515519</v>
+      </c>
+      <c r="O50" t="n">
+        <v>0.7181097405156232</v>
+      </c>
+      <c r="P50" t="n">
+        <v>0.3917627717418619</v>
+      </c>
+      <c r="Q50" t="n">
+        <v>0.3849273955872497</v>
+      </c>
+      <c r="R50" t="n">
+        <v>0.6800000000000002</v>
+      </c>
+      <c r="S50" t="n">
+        <v>0.6588235294117648</v>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51" t="n">
+        <v>51</v>
+      </c>
+      <c r="B51" t="n">
+        <v>0.25</v>
+      </c>
+      <c r="C51" t="n">
+        <v>0.25</v>
+      </c>
+      <c r="D51" t="n">
+        <v>0</v>
+      </c>
+      <c r="E51" t="n">
+        <v>0</v>
+      </c>
+      <c r="F51" t="n">
+        <v>0.25</v>
+      </c>
+      <c r="G51" t="n">
+        <v>0.25</v>
+      </c>
+      <c r="H51" t="n">
+        <v>0.163</v>
+      </c>
+      <c r="I51" t="n">
+        <v>0.021</v>
+      </c>
+      <c r="J51" t="n">
+        <v>0.83</v>
+      </c>
+      <c r="K51" t="n">
+        <v>0.08599999999999999</v>
+      </c>
+      <c r="L51" t="n">
+        <v>0.75</v>
+      </c>
+      <c r="M51" t="n">
+        <v>0.638</v>
+      </c>
+      <c r="N51" t="n">
+        <v>0.6456568963334186</v>
+      </c>
+      <c r="O51" t="n">
+        <v>0.7004956267791662</v>
+      </c>
+      <c r="P51" t="n">
+        <v>0.2069820897032919</v>
+      </c>
+      <c r="Q51" t="n">
+        <v>0.2</v>
+      </c>
+      <c r="R51" t="n">
+        <v>0.8</v>
+      </c>
+      <c r="S51" t="n">
+        <v>0.7294117647058822</v>
+      </c>
+    </row>
+    <row r="52">
+      <c r="A52" t="n">
+        <v>52</v>
+      </c>
+      <c r="B52" t="n">
+        <v>0.25</v>
+      </c>
+      <c r="C52" t="n">
+        <v>0</v>
+      </c>
+      <c r="D52" t="n">
+        <v>0.25</v>
+      </c>
+      <c r="E52" t="n">
+        <v>0</v>
+      </c>
+      <c r="F52" t="n">
+        <v>0.25</v>
+      </c>
+      <c r="G52" t="n">
+        <v>0.25</v>
+      </c>
+      <c r="H52" t="n">
+        <v>0.153</v>
+      </c>
+      <c r="I52" t="n">
+        <v>0.016</v>
+      </c>
+      <c r="J52" t="n">
+        <v>1.03</v>
+      </c>
+      <c r="K52" t="n">
+        <v>0.109</v>
+      </c>
+      <c r="L52" t="n">
+        <v>0.7</v>
+      </c>
+      <c r="M52" t="n">
+        <v>0.6</v>
+      </c>
+      <c r="N52" t="n">
+        <v>0.5992272042285747</v>
+      </c>
+      <c r="O52" t="n">
+        <v>0.6031454247400632</v>
+      </c>
+      <c r="P52" t="n">
+        <v>0.4147535773389229</v>
+      </c>
+      <c r="Q52" t="n">
+        <v>0.4153397346859768</v>
+      </c>
+      <c r="R52" t="n">
+        <v>0.6399999999999999</v>
+      </c>
+      <c r="S52" t="n">
+        <v>0.6235294117647059</v>
+      </c>
+    </row>
+    <row r="53">
+      <c r="A53" t="n">
+        <v>53</v>
+      </c>
+      <c r="B53" t="n">
+        <v>0</v>
+      </c>
+      <c r="C53" t="n">
+        <v>0.25</v>
+      </c>
+      <c r="D53" t="n">
+        <v>0.25</v>
+      </c>
+      <c r="E53" t="n">
+        <v>0</v>
+      </c>
+      <c r="F53" t="n">
+        <v>0.25</v>
+      </c>
+      <c r="G53" t="n">
+        <v>0.25</v>
+      </c>
+      <c r="H53" t="n">
+        <v>0.164</v>
+      </c>
+      <c r="I53" t="n">
+        <v>0.019</v>
+      </c>
+      <c r="J53" t="n">
+        <v>0.93</v>
+      </c>
+      <c r="K53" t="n">
+        <v>0.092</v>
+      </c>
+      <c r="L53" t="n">
+        <v>0.7</v>
+      </c>
+      <c r="M53" t="n">
+        <v>0.625</v>
+      </c>
+      <c r="N53" t="n">
+        <v>0.6493100643724039</v>
+      </c>
+      <c r="O53" t="n">
+        <v>0.6654747445948892</v>
+      </c>
+      <c r="P53" t="n">
+        <v>0.3120487790184461</v>
+      </c>
+      <c r="Q53" t="n">
+        <v>0.2584847730661084</v>
+      </c>
+      <c r="R53" t="n">
+        <v>0.6399999999999999</v>
+      </c>
+      <c r="S53" t="n">
+        <v>0.6941176470588235</v>
+      </c>
+    </row>
+    <row r="54">
+      <c r="A54" t="n">
+        <v>54</v>
+      </c>
+      <c r="B54" t="n">
+        <v>0.25</v>
+      </c>
+      <c r="C54" t="n">
+        <v>0</v>
+      </c>
+      <c r="D54" t="n">
+        <v>0</v>
+      </c>
+      <c r="E54" t="n">
+        <v>0.25</v>
+      </c>
+      <c r="F54" t="n">
+        <v>0.25</v>
+      </c>
+      <c r="G54" t="n">
+        <v>0.25</v>
+      </c>
+      <c r="H54" t="n">
+        <v>0.129</v>
+      </c>
+      <c r="I54" t="n">
+        <v>0.012</v>
+      </c>
+      <c r="J54" t="n">
+        <v>0.89</v>
+      </c>
+      <c r="K54" t="n">
+        <v>0.091</v>
+      </c>
+      <c r="L54" t="n">
+        <v>0.675</v>
+      </c>
+      <c r="M54" t="n">
+        <v>0.525</v>
+      </c>
+      <c r="N54" t="n">
+        <v>0.4821575603276989</v>
+      </c>
+      <c r="O54" t="n">
+        <v>0.5280976769945173</v>
+      </c>
+      <c r="P54" t="n">
+        <v>0.2752700905289024</v>
+      </c>
+      <c r="Q54" t="n">
+        <v>0.2455462397056674</v>
+      </c>
+      <c r="R54" t="n">
+        <v>0.5600000000000001</v>
+      </c>
+      <c r="S54" t="n">
+        <v>0.411764705882353</v>
+      </c>
+    </row>
+    <row r="55">
+      <c r="A55" t="n">
+        <v>55</v>
+      </c>
+      <c r="B55" t="n">
+        <v>0</v>
+      </c>
+      <c r="C55" t="n">
+        <v>0.25</v>
+      </c>
+      <c r="D55" t="n">
+        <v>0</v>
+      </c>
+      <c r="E55" t="n">
+        <v>0.25</v>
+      </c>
+      <c r="F55" t="n">
+        <v>0.25</v>
+      </c>
+      <c r="G55" t="n">
+        <v>0.25</v>
+      </c>
+      <c r="H55" t="n">
+        <v>0.14</v>
+      </c>
+      <c r="I55" t="n">
+        <v>0.012</v>
+      </c>
+      <c r="J55" t="n">
+        <v>1.01</v>
+      </c>
+      <c r="K55" t="n">
+        <v>0.097</v>
+      </c>
+      <c r="L55" t="n">
+        <v>0.65</v>
+      </c>
+      <c r="M55" t="n">
+        <v>0.5629999999999999</v>
+      </c>
+      <c r="N55" t="n">
+        <v>0.5338335004166566</v>
+      </c>
+      <c r="O55" t="n">
+        <v>0.5297157592107227</v>
+      </c>
+      <c r="P55" t="n">
+        <v>0.3959789239400368</v>
+      </c>
+      <c r="Q55" t="n">
+        <v>0.3013350931040962</v>
+      </c>
+      <c r="R55" t="n">
+        <v>0.4800000000000001</v>
+      </c>
+      <c r="S55" t="n">
+        <v>0.5176470588235293</v>
+      </c>
+    </row>
+    <row r="56">
+      <c r="A56" t="n">
+        <v>56</v>
+      </c>
+      <c r="B56" t="n">
+        <v>0</v>
+      </c>
+      <c r="C56" t="n">
+        <v>0</v>
+      </c>
+      <c r="D56" t="n">
+        <v>0.25</v>
+      </c>
+      <c r="E56" t="n">
+        <v>0.25</v>
+      </c>
+      <c r="F56" t="n">
+        <v>0.25</v>
+      </c>
+      <c r="G56" t="n">
+        <v>0.25</v>
+      </c>
+      <c r="H56" t="n">
+        <v>0.138</v>
+      </c>
+      <c r="I56" t="n">
+        <v>0.013</v>
+      </c>
+      <c r="J56" t="n">
+        <v>0.97</v>
+      </c>
+      <c r="K56" t="n">
+        <v>0.099</v>
+      </c>
+      <c r="L56" t="n">
+        <v>0.675</v>
+      </c>
+      <c r="M56" t="n">
+        <v>0.538</v>
+      </c>
+      <c r="N56" t="n">
+        <v>0.5252841218736706</v>
+      </c>
+      <c r="O56" t="n">
+        <v>0.5439815328111044</v>
+      </c>
+      <c r="P56" t="n">
+        <v>0.3590952682465028</v>
+      </c>
+      <c r="Q56" t="n">
+        <v>0.320967373283378</v>
+      </c>
+      <c r="R56" t="n">
+        <v>0.5600000000000001</v>
+      </c>
+      <c r="S56" t="n">
+        <v>0.4470588235294117</v>
+      </c>
+    </row>
+    <row r="57">
+      <c r="A57" t="n">
+        <v>57</v>
+      </c>
+      <c r="B57" t="n">
+        <v>0.2</v>
+      </c>
+      <c r="C57" t="n">
+        <v>0.2</v>
+      </c>
+      <c r="D57" t="n">
+        <v>0.2</v>
+      </c>
+      <c r="E57" t="n">
+        <v>0.2</v>
+      </c>
+      <c r="F57" t="n">
+        <v>0.2</v>
+      </c>
+      <c r="G57" t="n">
+        <v>0</v>
+      </c>
+      <c r="H57" t="n">
+        <v>0.172</v>
+      </c>
+      <c r="I57" t="n">
+        <v>0.02</v>
+      </c>
+      <c r="J57" t="n">
+        <v>1.01</v>
+      </c>
+      <c r="K57" t="n">
+        <v>0.102</v>
+      </c>
+      <c r="L57" t="n">
+        <v>0.713</v>
+      </c>
+      <c r="M57" t="n">
+        <v>0.6</v>
+      </c>
+      <c r="N57" t="n">
+        <v>0.6867365494143092</v>
+      </c>
+      <c r="O57" t="n">
+        <v>0.6731138601658053</v>
+      </c>
+      <c r="P57" t="n">
+        <v>0.4022017375436784</v>
+      </c>
+      <c r="Q57" t="n">
+        <v>0.3461817214148014</v>
+      </c>
+      <c r="R57" t="n">
+        <v>0.6800000000000002</v>
+      </c>
+      <c r="S57" t="n">
+        <v>0.6235294117647059</v>
+      </c>
+    </row>
+    <row r="58">
+      <c r="A58" t="n">
+        <v>58</v>
+      </c>
+      <c r="B58" t="n">
+        <v>0.2</v>
+      </c>
+      <c r="C58" t="n">
+        <v>0.2</v>
+      </c>
+      <c r="D58" t="n">
+        <v>0.2</v>
+      </c>
+      <c r="E58" t="n">
+        <v>0.2</v>
+      </c>
+      <c r="F58" t="n">
+        <v>0</v>
+      </c>
+      <c r="G58" t="n">
+        <v>0.2</v>
+      </c>
+      <c r="H58" t="n">
+        <v>0.181</v>
+      </c>
+      <c r="I58" t="n">
+        <v>0.023</v>
+      </c>
+      <c r="J58" t="n">
+        <v>0.96</v>
+      </c>
+      <c r="K58" t="n">
+        <v>0.105</v>
+      </c>
+      <c r="L58" t="n">
+        <v>0.675</v>
+      </c>
+      <c r="M58" t="n">
+        <v>0.575</v>
+      </c>
+      <c r="N58" t="n">
+        <v>0.7304478412449085</v>
+      </c>
+      <c r="O58" t="n">
+        <v>0.7436054552886897</v>
+      </c>
+      <c r="P58" t="n">
+        <v>0.3504734917373678</v>
+      </c>
+      <c r="Q58" t="n">
+        <v>0.3793533790302935</v>
+      </c>
+      <c r="R58" t="n">
+        <v>0.5600000000000001</v>
+      </c>
+      <c r="S58" t="n">
+        <v>0.552941176470588</v>
+      </c>
+    </row>
+    <row r="59">
+      <c r="A59" t="n">
+        <v>59</v>
+      </c>
+      <c r="B59" t="n">
+        <v>0.2</v>
+      </c>
+      <c r="C59" t="n">
+        <v>0.2</v>
+      </c>
+      <c r="D59" t="n">
+        <v>0.2</v>
+      </c>
+      <c r="E59" t="n">
+        <v>0</v>
+      </c>
+      <c r="F59" t="n">
+        <v>0.2</v>
+      </c>
+      <c r="G59" t="n">
+        <v>0.2</v>
+      </c>
+      <c r="H59" t="n">
+        <v>0.171</v>
+      </c>
+      <c r="I59" t="n">
+        <v>0.022</v>
+      </c>
+      <c r="J59" t="n">
+        <v>0.9399999999999999</v>
+      </c>
+      <c r="K59" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="L59" t="n">
+        <v>0.7</v>
+      </c>
+      <c r="M59" t="n">
+        <v>0.638</v>
+      </c>
+      <c r="N59" t="n">
+        <v>0.6853965922079943</v>
+      </c>
+      <c r="O59" t="n">
+        <v>0.7067919755818883</v>
+      </c>
+      <c r="P59" t="n">
+        <v>0.3228429085770043</v>
+      </c>
+      <c r="Q59" t="n">
+        <v>0.3294314684985411</v>
+      </c>
+      <c r="R59" t="n">
+        <v>0.6399999999999999</v>
+      </c>
+      <c r="S59" t="n">
+        <v>0.7294117647058822</v>
+      </c>
+    </row>
+    <row r="60">
+      <c r="A60" t="n">
+        <v>60</v>
+      </c>
+      <c r="B60" t="n">
+        <v>0.2</v>
+      </c>
+      <c r="C60" t="n">
+        <v>0.2</v>
+      </c>
+      <c r="D60" t="n">
+        <v>0</v>
+      </c>
+      <c r="E60" t="n">
+        <v>0.2</v>
+      </c>
+      <c r="F60" t="n">
+        <v>0.2</v>
+      </c>
+      <c r="G60" t="n">
+        <v>0.2</v>
+      </c>
+      <c r="H60" t="n">
+        <v>0.153</v>
+      </c>
+      <c r="I60" t="n">
+        <v>0.018</v>
+      </c>
+      <c r="J60" t="n">
+        <v>0.88</v>
+      </c>
+      <c r="K60" t="n">
+        <v>0.08699999999999999</v>
+      </c>
+      <c r="L60" t="n">
+        <v>0.725</v>
+      </c>
+      <c r="M60" t="n">
+        <v>0.638</v>
+      </c>
+      <c r="N60" t="n">
+        <v>0.5957861098223458</v>
+      </c>
+      <c r="O60" t="n">
+        <v>0.6315992991014117</v>
+      </c>
+      <c r="P60" t="n">
+        <v>0.2599521585271699</v>
+      </c>
+      <c r="Q60" t="n">
+        <v>0.2041558093138795</v>
+      </c>
+      <c r="R60" t="n">
+        <v>0.72</v>
+      </c>
+      <c r="S60" t="n">
+        <v>0.7294117647058822</v>
+      </c>
+    </row>
+    <row r="61">
+      <c r="A61" t="n">
+        <v>61</v>
+      </c>
+      <c r="B61" t="n">
+        <v>0.2</v>
+      </c>
+      <c r="C61" t="n">
+        <v>0</v>
+      </c>
+      <c r="D61" t="n">
+        <v>0.2</v>
+      </c>
+      <c r="E61" t="n">
+        <v>0.2</v>
+      </c>
+      <c r="F61" t="n">
+        <v>0.2</v>
+      </c>
+      <c r="G61" t="n">
+        <v>0.2</v>
+      </c>
+      <c r="H61" t="n">
+        <v>0.156</v>
+      </c>
+      <c r="I61" t="n">
+        <v>0.018</v>
+      </c>
+      <c r="J61" t="n">
+        <v>0.97</v>
+      </c>
+      <c r="K61" t="n">
+        <v>0.104</v>
+      </c>
+      <c r="L61" t="n">
+        <v>0.663</v>
+      </c>
+      <c r="M61" t="n">
+        <v>0.525</v>
+      </c>
+      <c r="N61" t="n">
+        <v>0.6125462900314183</v>
+      </c>
+      <c r="O61" t="n">
+        <v>0.6311191302751334</v>
+      </c>
+      <c r="P61" t="n">
+        <v>0.3597298411981057</v>
+      </c>
+      <c r="Q61" t="n">
+        <v>0.3689582281640068</v>
+      </c>
+      <c r="R61" t="n">
+        <v>0.5199999999999999</v>
+      </c>
+      <c r="S61" t="n">
+        <v>0.411764705882353</v>
+      </c>
+    </row>
+    <row r="62">
+      <c r="A62" t="n">
+        <v>62</v>
+      </c>
+      <c r="B62" t="n">
+        <v>0</v>
+      </c>
+      <c r="C62" t="n">
+        <v>0.2</v>
+      </c>
+      <c r="D62" t="n">
+        <v>0.2</v>
+      </c>
+      <c r="E62" t="n">
+        <v>0.2</v>
+      </c>
+      <c r="F62" t="n">
+        <v>0.2</v>
+      </c>
+      <c r="G62" t="n">
+        <v>0.2</v>
+      </c>
+      <c r="H62" t="n">
+        <v>0.161</v>
+      </c>
+      <c r="I62" t="n">
+        <v>0.018</v>
+      </c>
+      <c r="J62" t="n">
+        <v>0.98</v>
+      </c>
+      <c r="K62" t="n">
+        <v>0.094</v>
+      </c>
+      <c r="L62" t="n">
+        <v>0.6879999999999999</v>
+      </c>
+      <c r="M62" t="n">
+        <v>0.663</v>
+      </c>
+      <c r="N62" t="n">
+        <v>0.635785203959793</v>
+      </c>
+      <c r="O62" t="n">
+        <v>0.6344017609013193</v>
+      </c>
+      <c r="P62" t="n">
+        <v>0.3620387347733377</v>
+      </c>
+      <c r="Q62" t="n">
+        <v>0.2772206017793437</v>
+      </c>
+      <c r="R62" t="n">
+        <v>0.6</v>
+      </c>
+      <c r="S62" t="n">
+        <v>0.8</v>
+      </c>
+    </row>
+    <row r="63">
+      <c r="A63" t="n">
+        <v>63</v>
+      </c>
+      <c r="B63" t="n">
+        <v>0.167</v>
+      </c>
+      <c r="C63" t="n">
+        <v>0.167</v>
+      </c>
+      <c r="D63" t="n">
+        <v>0.167</v>
+      </c>
+      <c r="E63" t="n">
+        <v>0.167</v>
+      </c>
+      <c r="F63" t="n">
+        <v>0.167</v>
+      </c>
+      <c r="G63" t="n">
+        <v>0.167</v>
+      </c>
+      <c r="H63" t="n">
+        <v>0.173</v>
+      </c>
+      <c r="I63" t="n">
+        <v>0.022</v>
+      </c>
+      <c r="J63" t="n">
+        <v>0.91</v>
+      </c>
+      <c r="K63" t="n">
+        <v>0.095</v>
+      </c>
+      <c r="L63" t="n">
+        <v>0.713</v>
+      </c>
+      <c r="M63" t="n">
+        <v>0.663</v>
+      </c>
+      <c r="N63" t="n">
+        <v>0.6926919662189297</v>
+      </c>
+      <c r="O63" t="n">
+        <v>0.7164763582209457</v>
+      </c>
+      <c r="P63" t="n">
+        <v>0.2960737026978929</v>
+      </c>
+      <c r="Q63" t="n">
+        <v>0.2849232182788519</v>
+      </c>
+      <c r="R63" t="n">
+        <v>0.6800000000000002</v>
+      </c>
+      <c r="S63" t="n">
+        <v>0.8</v>
       </c>
     </row>
   </sheetData>
@@ -897,6 +4609,101 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:F3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>Model</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>Mean Squared Error</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>R-squared Score</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>Precision</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>Recall</t>
+        </is>
+      </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
+          <t>F1 Score</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>Linear Regression</t>
+        </is>
+      </c>
+      <c r="B2" t="n">
+        <v>0.008779620736781103</v>
+      </c>
+      <c r="C2" t="n">
+        <v>0.3113816683205967</v>
+      </c>
+      <c r="D2" t="n">
+        <v>0.6071428571428572</v>
+      </c>
+      <c r="E2" t="n">
+        <v>0.6125</v>
+      </c>
+      <c r="F2" t="n">
+        <v>0.606060606060606</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>Random Forest</t>
+        </is>
+      </c>
+      <c r="B3" t="n">
+        <v>0.002368600161810785</v>
+      </c>
+      <c r="C3" t="n">
+        <v>0.7396893446872636</v>
+      </c>
+      <c r="D3" t="n">
+        <v>0.8125</v>
+      </c>
+      <c r="E3" t="n">
+        <v>1</v>
+      </c>
+      <c r="F3" t="n">
+        <v>0.8846153846153846</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -2228,7 +6035,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>

</xml_diff>